<commit_message>
Login and Register Completed
</commit_message>
<xml_diff>
--- a/data/user_details.xlsx
+++ b/data/user_details.xlsx
@@ -1,63 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\python programs\__my programs\Train-ticket-booking-system\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB3E38B-CB9A-4A74-9049-42D65F4111BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>date of birth</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,8 +46,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -86,48 +56,108 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DA92786-951F-45BE-B4FC-3753878EFB57}" name="Table1" displayName="Table1" ref="A1:E594" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E594" xr:uid="{3EC62CA6-C929-44EB-97FD-A96C61D0FAB0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E594" headerRowCount="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E594"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{35E494DF-F7DB-4A20-8362-98CDCEEDA6B6}" name="Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{718D9A7A-17EA-4B6B-AEC7-EBAC963A622E}" name="Email" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{EDFCC637-A1D8-4D7F-B1D8-311F693A5F92}" name="gender" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B85BCC63-8184-4B96-8CA0-62829FF92561}" name="date of birth" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{058F21AC-490E-4E31-8276-F8C756DA4FAF}" name="password" dataDxfId="2"/>
+    <tableColumn id="1" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" name="Email" dataDxfId="3"/>
+    <tableColumn id="3" name="gender" dataDxfId="2"/>
+    <tableColumn id="4" name="date of birth" dataDxfId="1"/>
+    <tableColumn id="5" name="password" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -395,44 +425,247 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col width="22.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="19.7109375" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="18.140625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="17.85546875" customWidth="1" style="1" min="5" max="5"/>
+    <col width="9.140625" customWidth="1" style="1" min="6" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>date of birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mdi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>pabiadn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mdi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>pabi.adn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mdi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>pabi.adn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mdi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>pabi.adn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mdi</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>pabi.adn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>qw</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>pabi.adn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>mdi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>pabi.adn1@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>14/02/2021</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redid the login logic
</commit_message>
<xml_diff>
--- a/data/user_details.xlsx
+++ b/data/user_details.xlsx
@@ -1,58 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\python programs\__my programs\Train ticket booking system\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA0315A-9E57-4AA2-88F3-1007A235068D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="users" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>date of birth</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -67,17 +50,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -103,26 +90,86 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E594" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E594" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E594" headerRowCount="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E594"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Email" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="gender" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="date of birth" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="password" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" name="Email" dataDxfId="3"/>
+    <tableColumn id="3" name="gender" dataDxfId="2"/>
+    <tableColumn id="4" name="date of birth" dataDxfId="1"/>
+    <tableColumn id="5" name="password" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -390,73 +437,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="A2:E5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col width="22.5703125" customWidth="1" style="1" min="1" max="1"/>
+    <col width="28.28515625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="13.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="18.140625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="17.85546875" customWidth="1" style="1" min="5" max="5"/>
+    <col width="9.140625" customWidth="1" style="1" min="6" max="7"/>
+    <col width="9.140625" customWidth="1" style="1" min="8" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>date of birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Prakash</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>prakash218kumar@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>36912</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1234</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>prakash</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>johnsummerlin383@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>07/03/2021</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
+    <row r="4"/>
+    <row r="5"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>